<commit_message>
Added a new client
</commit_message>
<xml_diff>
--- a/Daily_Stats_L1_Support.xlsx
+++ b/Daily_Stats_L1_Support.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="63">
   <si>
     <t>Type</t>
   </si>
@@ -49,12 +49,21 @@
     <t>AMCN HIDIVE Client Support</t>
   </si>
   <si>
+    <t>Blast TV Client Support</t>
+  </si>
+  <si>
     <t>EuroLeague Client Support</t>
   </si>
   <si>
+    <t>Feyenoord Client Support</t>
+  </si>
+  <si>
     <t>NZ Rugby Client Support</t>
   </si>
   <si>
+    <t>Sport24 Client Support</t>
+  </si>
+  <si>
     <t>TNA Plus Client Support</t>
   </si>
   <si>
@@ -73,6 +82,9 @@
     <t>Dice Support Tickets</t>
   </si>
   <si>
+    <t>EuroLeague TV</t>
+  </si>
+  <si>
     <t>Melissa Wood Health</t>
   </si>
   <si>
@@ -82,6 +94,9 @@
     <t>Oilers Plus</t>
   </si>
   <si>
+    <t>Rugbypass.tv</t>
+  </si>
+  <si>
     <t>SkweekTV</t>
   </si>
   <si>
@@ -94,10 +109,7 @@
     <t>SuperLeague+</t>
   </si>
   <si>
-    <t>SuperMotocross Video Pass</t>
-  </si>
-  <si>
-    <t>TNA+</t>
+    <t>UFC</t>
   </si>
   <si>
     <t>SUM</t>
@@ -130,33 +142,36 @@
 Tickets</t>
   </si>
   <si>
-    <t>2025-05-12</t>
+    <t>2025-05-26</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>R &amp; A Client Support</t>
+    <t>ABFF Play</t>
   </si>
   <si>
     <t>Carlisle United TV</t>
   </si>
   <si>
-    <t>EuroLeague TV</t>
-  </si>
-  <si>
     <t>European League of Football</t>
   </si>
   <si>
     <t>Fever Direct</t>
   </si>
   <si>
+    <t>NZ Rugby</t>
+  </si>
+  <si>
+    <t>SuperMotocross Video Pass</t>
+  </si>
+  <si>
+    <t>TNA+</t>
+  </si>
+  <si>
     <t>UEFA TV</t>
   </si>
   <si>
-    <t>UFC</t>
-  </si>
-  <si>
     <t>UFC Fight Pass Brasil</t>
   </si>
   <si>
@@ -187,13 +202,13 @@
     <t>P2</t>
   </si>
   <si>
-    <t>2025-05-12T10:03:21</t>
-  </si>
-  <si>
-    <t>1403450</t>
-  </si>
-  <si>
-    <t>Need RCA - Esraa's account - need a security audit and root cause of account removal</t>
+    <t>2025-05-26T04:24:04</t>
+  </si>
+  <si>
+    <t>1408586</t>
+  </si>
+  <si>
+    <t>Mobile(TAB)_Regression_14.26.2(925): Unable to Enable Caps Lock on Login Screen.</t>
   </si>
 </sst>
 </file>
@@ -297,7 +312,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -360,7 +375,7 @@
         <v>8</v>
       </c>
       <c r="C5" t="n" s="0">
-        <v>70.0</v>
+        <v>74.0</v>
       </c>
     </row>
     <row r="6">
@@ -371,7 +386,7 @@
         <v>9</v>
       </c>
       <c r="C6" t="n" s="0">
-        <v>117.0</v>
+        <v>103.0</v>
       </c>
     </row>
     <row r="7">
@@ -382,7 +397,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="n" s="0">
-        <v>48.0</v>
+        <v>64.0</v>
       </c>
     </row>
     <row r="8">
@@ -401,10 +416,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C9" t="n" s="0">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="10">
@@ -412,7 +427,7 @@
         <v>7</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C10" t="n" s="0">
         <v>1.0</v>
@@ -423,10 +438,10 @@
         <v>7</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C11" t="n" s="0">
-        <v>19.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="12">
@@ -434,7 +449,7 @@
         <v>7</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C12" t="n" s="0">
         <v>1.0</v>
@@ -445,10 +460,10 @@
         <v>7</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C13" t="n" s="0">
-        <v>5.0</v>
+        <v>25.0</v>
       </c>
     </row>
     <row r="14">
@@ -470,7 +485,7 @@
         <v>16</v>
       </c>
       <c r="C15" t="n" s="0">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="16">
@@ -478,48 +493,48 @@
         <v>7</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C16" t="n" s="0">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B17" t="s" s="0">
         <v>18</v>
       </c>
       <c r="C17" t="n" s="0">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B18" t="s" s="0">
         <v>19</v>
       </c>
       <c r="C18" t="n" s="0">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C19" t="n" s="0">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s" s="0">
         <v>21</v>
@@ -530,51 +545,51 @@
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s" s="0">
         <v>22</v>
       </c>
       <c r="C21" t="n" s="0">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s" s="0">
         <v>23</v>
       </c>
       <c r="C22" t="n" s="0">
-        <v>43.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B23" t="s" s="0">
         <v>24</v>
       </c>
       <c r="C23" t="n" s="0">
-        <v>9.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B24" t="s" s="0">
         <v>25</v>
       </c>
       <c r="C24" t="n" s="0">
-        <v>16.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B25" t="s" s="0">
         <v>26</v>
@@ -585,24 +600,68 @@
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B26" t="s" s="0">
         <v>27</v>
       </c>
       <c r="C26" t="n" s="0">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B27" t="s" s="0">
         <v>28</v>
       </c>
       <c r="C27" t="n" s="0">
-        <v>358.0</v>
+        <v>51.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B28" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="C28" t="n" s="0">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B29" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="C29" t="n" s="0">
+        <v>20.0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B30" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="C30" t="n" s="0">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="B31" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="C31" t="n" s="0">
+        <v>388.0</v>
       </c>
     </row>
   </sheetData>
@@ -612,7 +671,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -620,7 +679,7 @@
   <cols>
     <col min="1" max="1" width="4.83984375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="10.0390625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="28.984375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="25.02734375" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="10.95703125" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="6.5625" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="6.5625" customWidth="true" bestFit="true"/>
@@ -634,28 +693,28 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="5">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C1" t="s" s="6">
         <v>1</v>
       </c>
       <c r="D1" t="s" s="7">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E1" t="s" s="8">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="F1" t="s" s="9">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="G1" t="s" s="10">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="H1" t="s" s="11">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="I1" t="s" s="12">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2">
@@ -663,25 +722,25 @@
         <v>7</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s" s="0">
         <v>8</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F2" t="n" s="0">
         <v>1.0</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="H2" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="I2" t="n" s="0">
         <v>1.0</v>
@@ -692,28 +751,28 @@
         <v>7</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>37</v>
-      </c>
-      <c r="F3" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
+      </c>
+      <c r="F3" t="n" s="0">
+        <v>4.0</v>
       </c>
       <c r="G3" t="s" s="0">
-        <v>37</v>
-      </c>
-      <c r="H3" t="n" s="0">
-        <v>6.0</v>
+        <v>41</v>
+      </c>
+      <c r="H3" t="s" s="0">
+        <v>41</v>
       </c>
       <c r="I3" t="n" s="0">
-        <v>6.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="4">
@@ -721,28 +780,28 @@
         <v>7</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F4" t="n" s="0">
         <v>1.0</v>
       </c>
       <c r="G4" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="H4" t="n" s="0">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="I4" t="n" s="0">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="5">
@@ -750,25 +809,25 @@
         <v>7</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>37</v>
-      </c>
-      <c r="F5" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
+      </c>
+      <c r="F5" t="n" s="0">
+        <v>1.0</v>
       </c>
       <c r="G5" t="s" s="0">
-        <v>37</v>
-      </c>
-      <c r="H5" t="n" s="0">
-        <v>1.0</v>
+        <v>41</v>
+      </c>
+      <c r="H5" t="s" s="0">
+        <v>41</v>
       </c>
       <c r="I5" t="n" s="0">
         <v>1.0</v>
@@ -776,28 +835,28 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>37</v>
-      </c>
-      <c r="F6" t="n" s="0">
+        <v>41</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="G6" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="H6" t="n" s="0">
         <v>2.0</v>
-      </c>
-      <c r="G6" t="s" s="0">
-        <v>37</v>
-      </c>
-      <c r="H6" t="s" s="0">
-        <v>37</v>
       </c>
       <c r="I6" t="n" s="0">
         <v>2.0</v>
@@ -805,28 +864,28 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="D7" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E7" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F7" t="n" s="0">
         <v>1.0</v>
       </c>
       <c r="G7" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="H7" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="I7" t="n" s="0">
         <v>1.0</v>
@@ -834,173 +893,173 @@
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s" s="0">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E8" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F8" t="n" s="0">
-        <v>2.0</v>
+        <v>13.0</v>
       </c>
       <c r="G8" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="H8" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="I8" t="n" s="0">
-        <v>2.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C9" t="s" s="0">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E9" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F9" t="n" s="0">
-        <v>4.0</v>
+        <v>78.0</v>
       </c>
       <c r="G9" t="s" s="0">
-        <v>37</v>
-      </c>
-      <c r="H9" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
+      </c>
+      <c r="H9" t="n" s="0">
+        <v>3.0</v>
       </c>
       <c r="I9" t="n" s="0">
-        <v>4.0</v>
+        <v>81.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s" s="0">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D10" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E10" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F10" t="n" s="0">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G10" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="H10" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="I10" t="n" s="0">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s" s="0">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="D11" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E11" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F11" t="n" s="0">
-        <v>7.0</v>
+        <v>1.0</v>
       </c>
       <c r="G11" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="H11" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="I11" t="n" s="0">
-        <v>7.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s" s="0">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="D12" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E12" t="s" s="0">
-        <v>37</v>
-      </c>
-      <c r="F12" t="n" s="0">
-        <v>16.0</v>
+        <v>41</v>
+      </c>
+      <c r="F12" t="s" s="0">
+        <v>41</v>
       </c>
       <c r="G12" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="H12" t="n" s="0">
         <v>1.0</v>
       </c>
       <c r="I12" t="n" s="0">
-        <v>17.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C13" t="s" s="0">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="D13" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E13" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F13" t="n" s="0">
         <v>1.0</v>
       </c>
       <c r="G13" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="H13" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="I13" t="n" s="0">
         <v>1.0</v>
@@ -1008,141 +1067,141 @@
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s" s="0">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="D14" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E14" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F14" t="n" s="0">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c r="G14" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="H14" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="I14" t="n" s="0">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C15" t="s" s="0">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="D15" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E15" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F15" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="G15" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="H15" t="n" s="0">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="I15" t="n" s="0">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C16" t="s" s="0">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D16" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E16" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F16" t="n" s="0">
-        <v>46.0</v>
-      </c>
-      <c r="G16" t="n" s="0">
-        <v>6.0</v>
-      </c>
-      <c r="H16" t="s" s="0">
-        <v>37</v>
+        <v>12.0</v>
+      </c>
+      <c r="G16" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="H16" t="n" s="0">
+        <v>1.0</v>
       </c>
       <c r="I16" t="n" s="0">
-        <v>52.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C17" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="D17" t="s" s="0">
-        <v>37</v>
+        <v>28</v>
+      </c>
+      <c r="D17" t="n" s="0">
+        <v>1.0</v>
       </c>
       <c r="E17" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F17" t="n" s="0">
-        <v>5.0</v>
-      </c>
-      <c r="G17" t="s" s="0">
-        <v>37</v>
+        <v>70.0</v>
+      </c>
+      <c r="G17" t="n" s="0">
+        <v>20.0</v>
       </c>
       <c r="H17" t="n" s="0">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="I17" t="n" s="0">
-        <v>6.0</v>
+        <v>94.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C18" t="s" s="0">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D18" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E18" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F18" t="n" s="0">
         <v>3.0</v>
       </c>
       <c r="G18" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="H18" t="n" s="0">
         <v>1.0</v>
@@ -1153,28 +1212,28 @@
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C19" t="s" s="0">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D19" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E19" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F19" t="n" s="0">
         <v>4.0</v>
       </c>
       <c r="G19" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="H19" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="I19" t="n" s="0">
         <v>4.0</v>
@@ -1182,176 +1241,234 @@
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C20" t="s" s="0">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D20" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E20" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F20" t="n" s="0">
         <v>1.0</v>
       </c>
       <c r="G20" t="s" s="0">
-        <v>37</v>
-      </c>
-      <c r="H20" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
+      </c>
+      <c r="H20" t="n" s="0">
+        <v>2.0</v>
       </c>
       <c r="I20" t="n" s="0">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C21" t="s" s="0">
-        <v>44</v>
-      </c>
-      <c r="D21" t="n" s="0">
-        <v>3.0</v>
-      </c>
-      <c r="E21" t="n" s="0">
-        <v>6.0</v>
+        <v>48</v>
+      </c>
+      <c r="D21" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="E21" t="s" s="0">
+        <v>41</v>
       </c>
       <c r="F21" t="n" s="0">
-        <v>34.0</v>
+        <v>2.0</v>
       </c>
       <c r="G21" t="s" s="0">
-        <v>37</v>
-      </c>
-      <c r="H21" t="n" s="0">
-        <v>12.0</v>
+        <v>41</v>
+      </c>
+      <c r="H21" t="s" s="0">
+        <v>41</v>
       </c>
       <c r="I21" t="n" s="0">
-        <v>55.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C22" t="s" s="0">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D22" t="s" s="0">
-        <v>37</v>
-      </c>
-      <c r="E22" t="n" s="0">
-        <v>18.0</v>
+        <v>41</v>
+      </c>
+      <c r="E22" t="s" s="0">
+        <v>41</v>
       </c>
       <c r="F22" t="n" s="0">
-        <v>20.0</v>
+        <v>3.0</v>
       </c>
       <c r="G22" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="H22" t="n" s="0">
-        <v>10.0</v>
+        <v>1.0</v>
       </c>
       <c r="I22" t="n" s="0">
-        <v>48.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C23" t="s" s="0">
-        <v>46</v>
-      </c>
-      <c r="D23" t="s" s="0">
-        <v>37</v>
-      </c>
-      <c r="E23" t="s" s="0">
-        <v>37</v>
+        <v>31</v>
+      </c>
+      <c r="D23" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="E23" t="n" s="0">
+        <v>6.0</v>
       </c>
       <c r="F23" t="n" s="0">
-        <v>6.0</v>
+        <v>24.0</v>
       </c>
       <c r="G23" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="H23" t="n" s="0">
-        <v>1.0</v>
+        <v>9.0</v>
       </c>
       <c r="I23" t="n" s="0">
-        <v>7.0</v>
+        <v>40.0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C24" t="s" s="0">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D24" t="s" s="0">
-        <v>37</v>
-      </c>
-      <c r="E24" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
+      </c>
+      <c r="E24" t="n" s="0">
+        <v>10.0</v>
       </c>
       <c r="F24" t="n" s="0">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="G24" t="s" s="0">
-        <v>37</v>
-      </c>
-      <c r="H24" t="s" s="0">
-        <v>37</v>
+        <v>41</v>
+      </c>
+      <c r="H24" t="n" s="0">
+        <v>2.0</v>
       </c>
       <c r="I24" t="n" s="0">
-        <v>11.0</v>
+        <v>22.0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="C25" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="D25" t="n" s="0">
-        <v>3.0</v>
-      </c>
-      <c r="E25" t="n" s="0">
-        <v>24.0</v>
+        <v>51</v>
+      </c>
+      <c r="D25" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="E25" t="s" s="0">
+        <v>41</v>
       </c>
       <c r="F25" t="n" s="0">
-        <v>168.0</v>
-      </c>
-      <c r="G25" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="G25" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="H25" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="I25" t="n" s="0">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B26" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="C26" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="D26" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="E26" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="F26" t="n" s="0">
         <v>6.0</v>
       </c>
-      <c r="H25" t="n" s="0">
-        <v>36.0</v>
-      </c>
-      <c r="I25" t="n" s="0">
-        <v>237.0</v>
+      <c r="G26" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="H26" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="I26" t="n" s="0">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="B27" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="C27" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D27" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="E27" t="n" s="0">
+        <v>16.0</v>
+      </c>
+      <c r="F27" t="n" s="0">
+        <v>248.0</v>
+      </c>
+      <c r="G27" t="n" s="0">
+        <v>20.0</v>
+      </c>
+      <c r="H27" t="n" s="0">
+        <v>30.0</v>
+      </c>
+      <c r="I27" t="n" s="0">
+        <v>316.0</v>
       </c>
     </row>
   </sheetData>
@@ -1370,50 +1487,50 @@
     <col min="1" max="1" width="10.625" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="17.94921875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="7.9140625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="21.10546875" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="70.7578125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="25.02734375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="69.1484375" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="15.265625" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="6.5625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="13">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s" s="14">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C1" t="s" s="15">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="D1" t="s" s="16">
         <v>1</v>
       </c>
       <c r="E1" t="s" s="17">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="F1" t="s" s="18">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="G1" t="s" s="19">
-        <v>53</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="F2" t="s" s="0">
         <v>3</v>

</xml_diff>

<commit_message>
removed ABFF from clients lists
</commit_message>
<xml_diff>
--- a/Daily_Stats_L1_Support.xlsx
+++ b/Daily_Stats_L1_Support.xlsx
@@ -8,13 +8,12 @@
   <sheets>
     <sheet name="Current Backlog" r:id="rId3" sheetId="1"/>
     <sheet name="Daily Support Contacts" r:id="rId4" sheetId="2"/>
-    <sheet name="Previous Day P1P2 Ticket..." r:id="rId5" sheetId="3"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="58">
   <si>
     <t>Type</t>
   </si>
@@ -25,12 +24,6 @@
     <t>Backlog Count</t>
   </si>
   <si>
-    <t> </t>
-  </si>
-  <si>
-    <t>Endeavor Streaming</t>
-  </si>
-  <si>
     <t>B2B</t>
   </si>
   <si>
@@ -49,6 +42,12 @@
     <t>BroadwayHD Client Support</t>
   </si>
   <si>
+    <t>Dallas Mavericks Client Support</t>
+  </si>
+  <si>
+    <t>EPL Client Support</t>
+  </si>
+  <si>
     <t>EuroLeague Client Support</t>
   </si>
   <si>
@@ -58,6 +57,9 @@
     <t>Longhorn Network Client Support</t>
   </si>
   <si>
+    <t>Melissa Wood Health Client Support</t>
+  </si>
+  <si>
     <t>NESN Client Support</t>
   </si>
   <si>
@@ -67,12 +69,12 @@
     <t>NZ Rugby Client Support</t>
   </si>
   <si>
-    <t>Pakistan Cricket Board Client Support</t>
-  </si>
-  <si>
     <t>Sky Sport Now Client Support</t>
   </si>
   <si>
+    <t>Spurs TV Client Support</t>
+  </si>
+  <si>
     <t>Supermotocross Client Support</t>
   </si>
   <si>
@@ -103,16 +105,22 @@
     <t>Dallas Mavericks TV</t>
   </si>
   <si>
-    <t>Dice Support Tickets</t>
-  </si>
-  <si>
     <t>EuroLeague TV</t>
   </si>
   <si>
+    <t>FIH</t>
+  </si>
+  <si>
     <t>Ligue 1+</t>
   </si>
   <si>
-    <t>Racer+</t>
+    <t>NZ Rugby</t>
+  </si>
+  <si>
+    <t>PCB Live</t>
+  </si>
+  <si>
+    <t>SkweekTV</t>
   </si>
   <si>
     <t>Sky Sport Now</t>
@@ -124,19 +132,13 @@
     <t>SuperLeague+</t>
   </si>
   <si>
-    <t>SuperMotocross Video Pass</t>
-  </si>
-  <si>
     <t>UFC</t>
   </si>
   <si>
     <t>UFC Fight Pass Brasil</t>
   </si>
   <si>
-    <t>Privacy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Endeavor Streaming Privacy </t>
+    <t>WWE Network</t>
   </si>
   <si>
     <t>SUM</t>
@@ -169,67 +171,28 @@
 Tickets</t>
   </si>
   <si>
-    <t>2025-10-15</t>
+    <t>2025-11-16</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>Melissa Wood Health</t>
-  </si>
-  <si>
-    <t>NZ Rugby</t>
-  </si>
-  <si>
-    <t>Oilers Plus</t>
-  </si>
-  <si>
-    <t>PCB Live</t>
-  </si>
-  <si>
-    <t>SkweekTV</t>
+    <t>Carlisle United TV</t>
+  </si>
+  <si>
+    <t>Dice Support Tickets</t>
+  </si>
+  <si>
+    <t>Endeavor Streaming</t>
+  </si>
+  <si>
+    <t>NWSL+</t>
   </si>
   <si>
     <t>TNA+</t>
   </si>
   <si>
     <t>Univision Now</t>
-  </si>
-  <si>
-    <t>Univision TVE</t>
-  </si>
-  <si>
-    <t>WWE Network</t>
-  </si>
-  <si>
-    <t>B2B Priority</t>
-  </si>
-  <si>
-    <t>Ticket Created</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Subject</t>
-  </si>
-  <si>
-    <t>Ticket external ID</t>
-  </si>
-  <si>
-    <t>Tickets</t>
-  </si>
-  <si>
-    <t>P2</t>
-  </si>
-  <si>
-    <t>2025-10-15T20:43:35</t>
-  </si>
-  <si>
-    <t>1497748</t>
-  </si>
-  <si>
-    <t>P1: NXT878_Ntwk - Not Processing in DVE</t>
   </si>
 </sst>
 </file>
@@ -266,30 +229,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
-      <alignment wrapText="true" vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
-      <alignment wrapText="true" vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
-      <alignment wrapText="true" vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
-      <alignment wrapText="true" vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
-      <alignment wrapText="true" vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
-      <alignment wrapText="true" vertical="center" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
-      <alignment wrapText="true" vertical="center" horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment wrapText="true" vertical="center" horizontal="center"/>
@@ -333,14 +275,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="6.74609375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="31.62890625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="4.83984375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="30.41015625" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="12.796875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
@@ -363,70 +305,70 @@
         <v>4</v>
       </c>
       <c r="C2" t="n" s="0">
-        <v>2.0</v>
+        <v>46.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="B3" t="s" s="0">
-        <v>6</v>
-      </c>
       <c r="C3" t="n" s="0">
-        <v>39.0</v>
+        <v>77.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" t="n" s="0">
-        <v>64.0</v>
+        <v>62.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" t="n" s="0">
-        <v>54.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" t="n" s="0">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" t="n" s="0">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" t="n" s="0">
         <v>1.0</v>
@@ -434,10 +376,10 @@
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" t="n" s="0">
         <v>1.0</v>
@@ -445,87 +387,87 @@
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" t="n" s="0">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" t="n" s="0">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" t="n" s="0">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" t="n" s="0">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" t="n" s="0">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C15" t="n" s="0">
-        <v>29.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16" t="n" s="0">
-        <v>1.0</v>
+        <v>39.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C17" t="n" s="0">
         <v>1.0</v>
@@ -533,10 +475,10 @@
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18" t="n" s="0">
         <v>1.0</v>
@@ -544,54 +486,54 @@
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C19" t="n" s="0">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C20" t="n" s="0">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C21" t="n" s="0">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C22" t="n" s="0">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C23" t="n" s="0">
         <v>1.0</v>
@@ -599,10 +541,10 @@
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="B24" t="s" s="0">
         <v>26</v>
-      </c>
-      <c r="B24" t="s" s="0">
-        <v>28</v>
       </c>
       <c r="C24" t="n" s="0">
         <v>1.0</v>
@@ -610,87 +552,87 @@
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C25" t="n" s="0">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C26" t="n" s="0">
-        <v>9.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C27" t="n" s="0">
-        <v>1.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C28" t="n" s="0">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C29" t="n" s="0">
-        <v>12.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C30" t="n" s="0">
-        <v>7.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C31" t="n" s="0">
-        <v>26.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C32" t="n" s="0">
         <v>1.0</v>
@@ -698,46 +640,79 @@
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C33" t="n" s="0">
-        <v>2.0</v>
+        <v>18.0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C34" t="n" s="0">
-        <v>2.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C35" t="n" s="0">
-        <v>1.0</v>
+        <v>26.0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="B36" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="C36" t="n" s="0">
+        <v>19.0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="B37" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="C37" t="n" s="0">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="B38" t="s" s="0">
         <v>41</v>
       </c>
-      <c r="B36" t="s" s="0">
-        <v>41</v>
-      </c>
-      <c r="C36" t="n" s="0">
-        <v>282.0</v>
+      <c r="C38" t="n" s="0">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="B39" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="C39" t="n" s="0">
+        <v>359.0</v>
       </c>
     </row>
   </sheetData>
@@ -747,15 +722,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="6.74609375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="4.83984375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="10.0390625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="24.49609375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="25.02734375" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="10.95703125" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="6.5625" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="6.5625" customWidth="true" bestFit="true"/>
@@ -769,141 +744,141 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="5">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C1" t="s" s="6">
         <v>1</v>
       </c>
       <c r="D1" t="s" s="7">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E1" t="s" s="8">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F1" t="s" s="9">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G1" t="s" s="10">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H1" t="s" s="11">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I1" t="s" s="12">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F2" t="n" s="0">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H2" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I2" t="n" s="0">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>50</v>
-      </c>
-      <c r="F3" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
+      </c>
+      <c r="F3" t="n" s="0">
+        <v>1.0</v>
       </c>
       <c r="G3" t="s" s="0">
-        <v>50</v>
-      </c>
-      <c r="H3" t="n" s="0">
-        <v>2.0</v>
+        <v>51</v>
+      </c>
+      <c r="H3" t="s" s="0">
+        <v>51</v>
       </c>
       <c r="I3" t="n" s="0">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F4" t="n" s="0">
-        <v>1.0</v>
+        <v>7.0</v>
       </c>
       <c r="G4" t="s" s="0">
-        <v>50</v>
-      </c>
-      <c r="H4" t="n" s="0">
-        <v>2.0</v>
+        <v>51</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>51</v>
       </c>
       <c r="I4" t="n" s="0">
-        <v>3.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F5" t="n" s="0">
         <v>1.0</v>
       </c>
       <c r="G5" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H5" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I5" t="n" s="0">
         <v>1.0</v>
@@ -911,492 +886,492 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>50</v>
-      </c>
-      <c r="F6" t="n" s="0">
-        <v>8.0</v>
+        <v>51</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>51</v>
       </c>
       <c r="G6" t="s" s="0">
-        <v>50</v>
-      </c>
-      <c r="H6" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
+      </c>
+      <c r="H6" t="n" s="0">
+        <v>3.0</v>
       </c>
       <c r="I6" t="n" s="0">
-        <v>8.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="D7" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E7" t="s" s="0">
-        <v>50</v>
-      </c>
-      <c r="F7" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
+      </c>
+      <c r="F7" t="n" s="0">
+        <v>1.0</v>
       </c>
       <c r="G7" t="s" s="0">
-        <v>50</v>
-      </c>
-      <c r="H7" t="n" s="0">
-        <v>6.0</v>
+        <v>51</v>
+      </c>
+      <c r="H7" t="s" s="0">
+        <v>51</v>
       </c>
       <c r="I7" t="n" s="0">
-        <v>6.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C8" t="s" s="0">
         <v>29</v>
       </c>
       <c r="D8" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E8" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F8" t="n" s="0">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G8" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H8" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I8" t="n" s="0">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C9" t="s" s="0">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="D9" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E9" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F9" t="n" s="0">
-        <v>62.0</v>
-      </c>
-      <c r="G9" t="n" s="0">
-        <v>7.0</v>
-      </c>
-      <c r="H9" t="n" s="0">
-        <v>2.0</v>
+        <v>1.0</v>
+      </c>
+      <c r="G9" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="H9" t="s" s="0">
+        <v>51</v>
       </c>
       <c r="I9" t="n" s="0">
-        <v>71.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C10" t="s" s="0">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="D10" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E10" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F10" t="n" s="0">
-        <v>78.0</v>
+        <v>1.0</v>
       </c>
       <c r="G10" t="s" s="0">
-        <v>50</v>
-      </c>
-      <c r="H10" t="n" s="0">
-        <v>4.0</v>
+        <v>51</v>
+      </c>
+      <c r="H10" t="s" s="0">
+        <v>51</v>
       </c>
       <c r="I10" t="n" s="0">
-        <v>82.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C11" t="s" s="0">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="D11" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E11" t="s" s="0">
-        <v>50</v>
-      </c>
-      <c r="F11" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
+      </c>
+      <c r="F11" t="n" s="0">
+        <v>16.0</v>
       </c>
       <c r="G11" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H11" t="n" s="0">
         <v>2.0</v>
       </c>
       <c r="I11" t="n" s="0">
-        <v>2.0</v>
+        <v>18.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C12" t="s" s="0">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E12" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F12" t="n" s="0">
+        <v>53.0</v>
+      </c>
+      <c r="G12" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="H12" t="n" s="0">
         <v>3.0</v>
       </c>
-      <c r="G12" t="s" s="0">
-        <v>50</v>
-      </c>
-      <c r="H12" t="s" s="0">
-        <v>50</v>
-      </c>
       <c r="I12" t="n" s="0">
-        <v>3.0</v>
+        <v>56.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C13" t="s" s="0">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D13" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E13" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F13" t="n" s="0">
-        <v>9.0</v>
+        <v>3.0</v>
       </c>
       <c r="G13" t="s" s="0">
-        <v>50</v>
-      </c>
-      <c r="H13" t="n" s="0">
-        <v>1.0</v>
+        <v>51</v>
+      </c>
+      <c r="H13" t="s" s="0">
+        <v>51</v>
       </c>
       <c r="I13" t="n" s="0">
-        <v>10.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C14" t="s" s="0">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="D14" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E14" t="s" s="0">
-        <v>50</v>
-      </c>
-      <c r="F14" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
+      </c>
+      <c r="F14" t="n" s="0">
+        <v>3.0</v>
       </c>
       <c r="G14" t="s" s="0">
-        <v>50</v>
-      </c>
-      <c r="H14" t="n" s="0">
-        <v>1.0</v>
+        <v>51</v>
+      </c>
+      <c r="H14" t="s" s="0">
+        <v>51</v>
       </c>
       <c r="I14" t="n" s="0">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C15" t="s" s="0">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D15" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E15" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F15" t="n" s="0">
         <v>1.0</v>
       </c>
       <c r="G15" t="s" s="0">
-        <v>50</v>
-      </c>
-      <c r="H15" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
+      </c>
+      <c r="H15" t="n" s="0">
+        <v>1.0</v>
       </c>
       <c r="I15" t="n" s="0">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C16" t="s" s="0">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="D16" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E16" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F16" t="n" s="0">
-        <v>31.0</v>
+        <v>1.0</v>
       </c>
       <c r="G16" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H16" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I16" t="n" s="0">
-        <v>31.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C17" t="s" s="0">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D17" t="n" s="0">
         <v>2.0</v>
       </c>
       <c r="E17" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F17" t="n" s="0">
-        <v>65.0</v>
+        <v>57.0</v>
       </c>
       <c r="G17" t="n" s="0">
-        <v>14.0</v>
+        <v>22.0</v>
       </c>
       <c r="H17" t="n" s="0">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
       <c r="I17" t="n" s="0">
-        <v>86.0</v>
+        <v>83.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C18" t="s" s="0">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D18" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E18" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F18" t="n" s="0">
-        <v>24.0</v>
+        <v>13.0</v>
       </c>
       <c r="G18" t="s" s="0">
-        <v>50</v>
-      </c>
-      <c r="H18" t="n" s="0">
-        <v>1.0</v>
+        <v>51</v>
+      </c>
+      <c r="H18" t="s" s="0">
+        <v>51</v>
       </c>
       <c r="I18" t="n" s="0">
-        <v>25.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C19" t="s" s="0">
         <v>56</v>
       </c>
       <c r="D19" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E19" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F19" t="n" s="0">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="G19" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H19" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I19" t="n" s="0">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C20" t="s" s="0">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D20" t="n" s="0">
-        <v>5.0</v>
+        <v>8.0</v>
       </c>
       <c r="E20" t="n" s="0">
-        <v>16.0</v>
+        <v>109.0</v>
       </c>
       <c r="F20" t="n" s="0">
+        <v>1397.0</v>
+      </c>
+      <c r="G20" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="H20" t="n" s="0">
         <v>23.0</v>
       </c>
-      <c r="G20" t="s" s="0">
-        <v>50</v>
-      </c>
-      <c r="H20" t="n" s="0">
-        <v>7.0</v>
-      </c>
       <c r="I20" t="n" s="0">
-        <v>51.0</v>
+        <v>1537.0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C21" t="s" s="0">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D21" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E21" t="n" s="0">
-        <v>25.0</v>
+        <v>520.0</v>
       </c>
       <c r="F21" t="n" s="0">
-        <v>17.0</v>
+        <v>351.0</v>
       </c>
       <c r="G21" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H21" t="n" s="0">
-        <v>8.0</v>
+        <v>72.0</v>
       </c>
       <c r="I21" t="n" s="0">
-        <v>50.0</v>
+        <v>943.0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C22" t="s" s="0">
         <v>57</v>
       </c>
       <c r="D22" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E22" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F22" t="n" s="0">
-        <v>9.0</v>
+        <v>11.0</v>
       </c>
       <c r="G22" t="s" s="0">
-        <v>50</v>
-      </c>
-      <c r="H22" t="n" s="0">
-        <v>2.0</v>
+        <v>51</v>
+      </c>
+      <c r="H22" t="s" s="0">
+        <v>51</v>
       </c>
       <c r="I22" t="n" s="0">
         <v>11.0</v>
@@ -1404,186 +1379,60 @@
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C23" t="s" s="0">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="D23" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E23" t="s" s="0">
-        <v>50</v>
-      </c>
-      <c r="F23" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
+      </c>
+      <c r="F23" t="n" s="0">
+        <v>6.0</v>
       </c>
       <c r="G23" t="s" s="0">
-        <v>50</v>
-      </c>
-      <c r="H23" t="n" s="0">
-        <v>2.0</v>
+        <v>51</v>
+      </c>
+      <c r="H23" t="s" s="0">
+        <v>51</v>
       </c>
       <c r="I23" t="n" s="0">
-        <v>2.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C24" t="s" s="0">
-        <v>59</v>
-      </c>
-      <c r="D24" t="s" s="0">
-        <v>50</v>
-      </c>
-      <c r="E24" t="s" s="0">
-        <v>50</v>
+        <v>42</v>
+      </c>
+      <c r="D24" t="n" s="0">
+        <v>10.0</v>
+      </c>
+      <c r="E24" t="n" s="0">
+        <v>629.0</v>
       </c>
       <c r="F24" t="n" s="0">
-        <v>14.0</v>
-      </c>
-      <c r="G24" t="s" s="0">
-        <v>50</v>
-      </c>
-      <c r="H24" t="s" s="0">
-        <v>50</v>
+        <v>1928.0</v>
+      </c>
+      <c r="G24" t="n" s="0">
+        <v>22.0</v>
+      </c>
+      <c r="H24" t="n" s="0">
+        <v>106.0</v>
       </c>
       <c r="I24" t="n" s="0">
-        <v>14.0</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s" s="0">
-        <v>39</v>
-      </c>
-      <c r="B25" t="s" s="0">
-        <v>49</v>
-      </c>
-      <c r="C25" t="s" s="0">
-        <v>40</v>
-      </c>
-      <c r="D25" t="s" s="0">
-        <v>50</v>
-      </c>
-      <c r="E25" t="s" s="0">
-        <v>50</v>
-      </c>
-      <c r="F25" t="n" s="0">
-        <v>1.0</v>
-      </c>
-      <c r="G25" t="s" s="0">
-        <v>50</v>
-      </c>
-      <c r="H25" t="s" s="0">
-        <v>50</v>
-      </c>
-      <c r="I25" t="n" s="0">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="s" s="0">
-        <v>41</v>
-      </c>
-      <c r="B26" t="s" s="0">
-        <v>41</v>
-      </c>
-      <c r="C26" t="s" s="0">
-        <v>41</v>
-      </c>
-      <c r="D26" t="n" s="0">
-        <v>7.0</v>
-      </c>
-      <c r="E26" t="n" s="0">
-        <v>41.0</v>
-      </c>
-      <c r="F26" t="n" s="0">
-        <v>355.0</v>
-      </c>
-      <c r="G26" t="n" s="0">
-        <v>21.0</v>
-      </c>
-      <c r="H26" t="n" s="0">
-        <v>45.0</v>
-      </c>
-      <c r="I26" t="n" s="0">
-        <v>469.0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <cols>
-    <col min="1" max="1" width="10.625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="17.94921875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="7.9140625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="17.3515625" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="34.890625" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="15.265625" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="6.5625" customWidth="true" bestFit="true"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="13">
-        <v>60</v>
-      </c>
-      <c r="B1" t="s" s="14">
-        <v>61</v>
-      </c>
-      <c r="C1" t="s" s="15">
-        <v>62</v>
-      </c>
-      <c r="D1" t="s" s="16">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s" s="17">
-        <v>63</v>
-      </c>
-      <c r="F1" t="s" s="18">
-        <v>64</v>
-      </c>
-      <c r="G1" t="s" s="19">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s" s="0">
-        <v>66</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>67</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>68</v>
-      </c>
-      <c r="D2" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="E2" t="s" s="0">
-        <v>69</v>
-      </c>
-      <c r="F2" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="G2" t="n" s="0">
-        <v>1.0</v>
+        <v>2695.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>